<commit_message>
Add solution problem 10
</commit_message>
<xml_diff>
--- a/others/stats.xlsx
+++ b/others/stats.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="19560" windowHeight="8340"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="19560" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="6">
   <si>
     <t>2*</t>
   </si>
@@ -813,31 +814,31 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>19552</c:v>
+                  <c:v>20841</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12381</c:v>
+                  <c:v>13273</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9585</c:v>
+                  <c:v>10333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7955</c:v>
+                  <c:v>8649</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7109</c:v>
+                  <c:v>7826</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5113</c:v>
+                  <c:v>5745</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2928</c:v>
+                  <c:v>3500</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2442</c:v>
+                  <c:v>3186</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>2165</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -901,11 +902,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="254761584"/>
-        <c:axId val="254762704"/>
+        <c:axId val="187635904"/>
+        <c:axId val="187636464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="254761584"/>
+        <c:axId val="187635904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -1016,13 +1017,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254762704"/>
+        <c:crossAx val="187636464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="254762704"/>
+        <c:axId val="187636464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1135,7 +1136,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254761584"/>
+        <c:crossAx val="187635904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1766,16 +1767,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
+      <xdr:colOff>600075</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>114301</xdr:rowOff>
+      <xdr:rowOff>123826</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2063,7 +2064,7 @@
   <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T18" sqref="T18"/>
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2109,14 +2110,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="5">
-        <v>14849</v>
+        <v>15867</v>
       </c>
       <c r="C2" s="6">
-        <v>4703</v>
+        <v>4974</v>
       </c>
       <c r="D2" s="12">
         <f>B2+C2</f>
-        <v>19552</v>
+        <v>20841</v>
       </c>
       <c r="E2" s="22" t="s">
         <v>4</v>
@@ -2142,18 +2143,18 @@
         <v>2</v>
       </c>
       <c r="B3" s="4">
-        <v>10840</v>
+        <v>11637</v>
       </c>
       <c r="C3" s="3">
-        <v>1541</v>
+        <v>1636</v>
       </c>
       <c r="D3" s="13">
         <f t="shared" ref="D3:D26" si="0">B3+C3</f>
-        <v>12381</v>
+        <v>13273</v>
       </c>
       <c r="E3" s="23">
         <f>-(1-(D3/D2))</f>
-        <v>-0.36676554828150576</v>
+        <v>-0.363130368024567</v>
       </c>
       <c r="F3" s="28"/>
       <c r="G3" s="28"/>
@@ -2176,18 +2177,18 @@
         <v>3</v>
       </c>
       <c r="B4" s="4">
-        <v>8723</v>
+        <v>9386</v>
       </c>
       <c r="C4" s="3">
-        <v>862</v>
+        <v>947</v>
       </c>
       <c r="D4" s="13">
         <f t="shared" si="0"/>
-        <v>9585</v>
+        <v>10333</v>
       </c>
       <c r="E4" s="23">
-        <f t="shared" ref="E4:E9" si="1">-(1-(D4/D3))</f>
-        <v>-0.22582990065422825</v>
+        <f t="shared" ref="E4:E10" si="1">-(1-(D4/D3))</f>
+        <v>-0.22150229789798836</v>
       </c>
       <c r="F4" s="28"/>
       <c r="G4" s="28"/>
@@ -2210,18 +2211,18 @@
         <v>4</v>
       </c>
       <c r="B5" s="4">
-        <v>7575</v>
+        <v>8231</v>
       </c>
       <c r="C5" s="3">
-        <v>380</v>
+        <v>418</v>
       </c>
       <c r="D5" s="13">
         <f t="shared" si="0"/>
-        <v>7955</v>
+        <v>8649</v>
       </c>
       <c r="E5" s="23">
         <f t="shared" si="1"/>
-        <v>-0.17005738132498693</v>
+        <v>-0.1629729991290042</v>
       </c>
       <c r="F5" s="28"/>
       <c r="G5" s="28"/>
@@ -2244,18 +2245,18 @@
         <v>5</v>
       </c>
       <c r="B6" s="4">
-        <v>5953</v>
+        <v>6558</v>
       </c>
       <c r="C6" s="3">
-        <v>1156</v>
+        <v>1268</v>
       </c>
       <c r="D6" s="13">
         <f t="shared" si="0"/>
-        <v>7109</v>
+        <v>7826</v>
       </c>
       <c r="E6" s="23">
         <f t="shared" si="1"/>
-        <v>-0.10634820867379002</v>
+        <v>-9.5155509307434438E-2</v>
       </c>
       <c r="F6" s="28"/>
       <c r="G6" s="28"/>
@@ -2278,18 +2279,18 @@
         <v>6</v>
       </c>
       <c r="B7" s="4">
-        <v>4905</v>
+        <v>5498</v>
       </c>
       <c r="C7" s="3">
-        <v>208</v>
+        <v>247</v>
       </c>
       <c r="D7" s="13">
         <f t="shared" si="0"/>
-        <v>5113</v>
+        <v>5745</v>
       </c>
       <c r="E7" s="23">
         <f t="shared" si="1"/>
-        <v>-0.28077085384723588</v>
+        <v>-0.26590851009455663</v>
       </c>
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
@@ -2312,18 +2313,18 @@
         <v>7</v>
       </c>
       <c r="B8" s="4">
-        <v>2825</v>
+        <v>3372</v>
       </c>
       <c r="C8" s="3">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="D8" s="13">
         <f t="shared" si="0"/>
-        <v>2928</v>
+        <v>3500</v>
       </c>
       <c r="E8" s="23">
         <f t="shared" si="1"/>
-        <v>-0.42734206923528262</v>
+        <v>-0.3907745865970409</v>
       </c>
       <c r="F8" s="28"/>
       <c r="G8" s="28"/>
@@ -2346,18 +2347,18 @@
         <v>8</v>
       </c>
       <c r="B9" s="4">
-        <v>2242</v>
+        <v>3009</v>
       </c>
       <c r="C9" s="3">
-        <v>200</v>
+        <v>177</v>
       </c>
       <c r="D9" s="13">
         <f t="shared" si="0"/>
-        <v>2442</v>
+        <v>3186</v>
       </c>
       <c r="E9" s="23">
         <f t="shared" si="1"/>
-        <v>-0.16598360655737709</v>
+        <v>-8.9714285714285746E-2</v>
       </c>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
@@ -2380,17 +2381,18 @@
         <v>9</v>
       </c>
       <c r="B10" s="4">
-        <v>0</v>
+        <v>2110</v>
       </c>
       <c r="C10" s="3">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="D10" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E10" s="24" t="s">
-        <v>4</v>
+        <v>2165</v>
+      </c>
+      <c r="E10" s="23">
+        <f t="shared" si="1"/>
+        <v>-0.32046453232893912</v>
       </c>
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
@@ -2942,15 +2944,15 @@
       </c>
       <c r="B27" s="18">
         <f>SUM(B2:B26)</f>
-        <v>57912</v>
+        <v>65668</v>
       </c>
       <c r="C27" s="19">
         <f t="shared" ref="C27:D27" si="2">SUM(C2:C26)</f>
-        <v>9153</v>
+        <v>9850</v>
       </c>
       <c r="D27" s="20">
         <f t="shared" si="2"/>
-        <v>67065</v>
+        <v>75518</v>
       </c>
       <c r="E27" s="21"/>
       <c r="F27" s="28"/>
@@ -2974,4 +2976,16 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>